<commit_message>
update results reference cases
</commit_message>
<xml_diff>
--- a/use_cases/LWR_FT_2023/run/results.xlsx
+++ b/use_cases/LWR_FT_2023/run/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/LWR_FT_2023/run/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90171983-B2F1-2744-B33D-2524D757544C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F3E156-D1A8-C042-AA9F-46BB6006377B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="arma validation" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="191">
   <si>
     <t>Braidwood</t>
   </si>
@@ -446,12 +446,6 @@
     <t>covid</t>
   </si>
   <si>
-    <t>braidwood_capex_0.75</t>
-  </si>
-  <si>
-    <t>braidwood_capex_1.25</t>
-  </si>
-  <si>
     <t>braidwood_sweep</t>
   </si>
   <si>
@@ -461,12 +455,6 @@
     <t>nebraska</t>
   </si>
   <si>
-    <t>cooper_capex_0.75</t>
-  </si>
-  <si>
-    <t>cooper_capex_1.25</t>
-  </si>
-  <si>
     <t>cooper_sweep</t>
   </si>
   <si>
@@ -476,12 +464,6 @@
     <t>ohio</t>
   </si>
   <si>
-    <t>davis_besse_capex_0.75</t>
-  </si>
-  <si>
-    <t>davis_besse_capex_1.25</t>
-  </si>
-  <si>
     <t>davis_besse_sweep</t>
   </si>
   <si>
@@ -491,12 +473,6 @@
     <t>minnesota</t>
   </si>
   <si>
-    <t>prairie_island_capex_0.75</t>
-  </si>
-  <si>
-    <t>prairie_island_capex_1.25</t>
-  </si>
-  <si>
     <t>prairie_island_sweep</t>
   </si>
   <si>
@@ -506,12 +482,6 @@
     <t>west_south_central</t>
   </si>
   <si>
-    <t>stp_capex_0.75</t>
-  </si>
-  <si>
-    <t>stp_capex_1.25</t>
-  </si>
-  <si>
     <t>stp_sweep</t>
   </si>
   <si>
@@ -630,6 +600,18 @@
   </si>
   <si>
     <t>c</t>
+  </si>
+  <si>
+    <t>h2_import_capacity</t>
+  </si>
+  <si>
+    <t>h2_export_capacity</t>
+  </si>
+  <si>
+    <t>% total revenues from PTC</t>
+  </si>
+  <si>
+    <t>% total cost for cO2</t>
   </si>
 </sst>
 </file>
@@ -858,7 +840,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
@@ -873,7 +855,6 @@
     <xf numFmtId="1" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -885,6 +866,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -905,7 +889,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1029,19 +1014,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>20983988.333636161</c:v>
+                    <c:v>21033677.934552897</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>59328864.424743213</c:v>
+                    <c:v>59715548.340558067</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>488703.81705399998</c:v>
+                    <c:v>49325.395239999998</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1107963.5922518366</c:v>
+                    <c:v>1107938.389021104</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>237675596.92948309</c:v>
+                    <c:v>174310501.6662392</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1053,19 +1038,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>20983988.333636161</c:v>
+                    <c:v>21033677.934552897</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>59328864.424743213</c:v>
+                    <c:v>59715548.340558067</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>488703.81705399998</c:v>
+                    <c:v>49325.395239999998</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1107963.5922518366</c:v>
+                    <c:v>1107938.389021104</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>237675596.92948309</c:v>
+                    <c:v>174310501.6662392</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1114,19 +1099,19 @@
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1026673178.2199998</c:v>
+                  <c:v>974521482.11999989</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>882568681.06000006</c:v>
+                  <c:v>761023865.84000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>595602343.78000021</c:v>
+                  <c:v>544202455.4000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>923016535.61800003</c:v>
+                  <c:v>910353321.898</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>356157446</c:v>
+                  <c:v>-223366239.48000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4169,63 +4154,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="22"/>
-      <c r="B1" s="24" t="s">
+      <c r="A1" s="24"/>
+      <c r="B1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="24" t="s">
+      <c r="C1" s="27"/>
+      <c r="D1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="26" t="s">
+      <c r="E1" s="27"/>
+      <c r="F1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="27"/>
-      <c r="H1" s="24" t="s">
+      <c r="G1" s="29"/>
+      <c r="H1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="20" t="s">
+      <c r="I1" s="27"/>
+      <c r="J1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="21"/>
+      <c r="K1" s="23"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="23"/>
-      <c r="B2" s="13" t="s">
+      <c r="A2" s="25"/>
+      <c r="B2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="12" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="7">
@@ -4240,10 +4225,10 @@
       <c r="E3" s="7">
         <v>25.54626235988728</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="13">
         <v>32.977089999999997</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="13">
         <v>32.980620000000002</v>
       </c>
       <c r="H3" s="7">
@@ -4252,15 +4237,15 @@
       <c r="I3" s="7">
         <v>9.375560755254849</v>
       </c>
-      <c r="J3" s="14">
+      <c r="J3" s="13">
         <v>41.194870000000002</v>
       </c>
-      <c r="K3" s="15">
+      <c r="K3" s="14">
         <v>41.570810000000002</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="7">
@@ -4275,10 +4260,10 @@
       <c r="E4" s="7">
         <v>110.57936084123359</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="13">
         <v>23.072469999999999</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="13">
         <v>23.11992</v>
       </c>
       <c r="H4" s="7">
@@ -4287,15 +4272,15 @@
       <c r="I4" s="7">
         <v>15.06729275093023</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J4" s="13">
         <v>290.6533</v>
       </c>
-      <c r="K4" s="15">
+      <c r="K4" s="14">
         <v>290.52300000000002</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="7">
@@ -4310,10 +4295,10 @@
       <c r="E5" s="7">
         <v>-65.109300000000005</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="13">
         <v>2.27</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="13">
         <v>2.27</v>
       </c>
       <c r="H5" s="7">
@@ -4322,15 +4307,15 @@
       <c r="I5" s="7">
         <v>-66.2</v>
       </c>
-      <c r="J5" s="14">
+      <c r="J5" s="13">
         <v>-20.2</v>
       </c>
-      <c r="K5" s="15">
+      <c r="K5" s="14">
         <v>-20.2</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="7">
@@ -4345,10 +4330,10 @@
       <c r="E6" s="7">
         <v>14.37777231055</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="13">
         <v>22.72</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="13">
         <v>22.64517</v>
       </c>
       <c r="H6" s="7">
@@ -4357,15 +4342,15 @@
       <c r="I6" s="7">
         <v>-0.57533928877825002</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="13">
         <v>18.850000000000001</v>
       </c>
-      <c r="K6" s="15">
+      <c r="K6" s="14">
         <v>16.82328</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="7">
@@ -4380,10 +4365,10 @@
       <c r="E7" s="7">
         <v>19.173366480049999</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="13">
         <v>28.84</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="13">
         <v>28.829719999999998</v>
       </c>
       <c r="H7" s="7">
@@ -4392,15 +4377,15 @@
       <c r="I7" s="7">
         <v>0.58024959424</v>
       </c>
-      <c r="J7" s="14">
+      <c r="J7" s="13">
         <v>23.93</v>
       </c>
-      <c r="K7" s="15">
+      <c r="K7" s="14">
         <v>24.394089999999998</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="7">
@@ -4415,10 +4400,10 @@
       <c r="E8" s="7">
         <v>27.222851138425</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="13">
         <v>37</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="13">
         <v>37.050960000000003</v>
       </c>
       <c r="H8" s="7">
@@ -4427,15 +4412,15 @@
       <c r="I8" s="7">
         <v>21.463601906800001</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="13">
         <v>32.020000000000003</v>
       </c>
-      <c r="K8" s="15">
+      <c r="K8" s="14">
         <v>36.356409999999997</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="7">
@@ -4450,10 +4435,10 @@
       <c r="E9" s="7">
         <v>4230.9575999999997</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="13">
         <v>933.68</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="13">
         <v>933.68</v>
       </c>
       <c r="H9" s="7">
@@ -4462,15 +4447,15 @@
       <c r="I9" s="7">
         <v>97</v>
       </c>
-      <c r="J9" s="14">
+      <c r="J9" s="13">
         <v>8996.83</v>
       </c>
-      <c r="K9" s="15">
+      <c r="K9" s="14">
         <v>8996.83</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="7">
@@ -4485,10 +4470,10 @@
       <c r="E10" s="7">
         <v>749.96335094363985</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="13">
         <v>243.29750000000001</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="13">
         <v>241.2045</v>
       </c>
       <c r="H10" s="7">
@@ -4497,45 +4482,45 @@
       <c r="I10" s="7">
         <v>1.2223387323406909</v>
       </c>
-      <c r="J10" s="14">
+      <c r="J10" s="13">
         <v>699.61369999999999</v>
       </c>
-      <c r="K10" s="15">
+      <c r="K10" s="14">
         <v>696.71950000000004</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="15">
         <v>10.85681406844434</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="15">
         <v>10.81196311074452</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="15">
         <v>26.76559217679149</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="15">
         <v>26.607204309125571</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="16">
         <v>10.856809999999999</v>
       </c>
-      <c r="G11" s="17">
+      <c r="G11" s="16">
         <v>10.79345</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11" s="15">
         <v>1.292473562594213</v>
       </c>
-      <c r="I11" s="16">
+      <c r="I11" s="15">
         <v>1.297771260495596</v>
       </c>
-      <c r="J11" s="17">
+      <c r="J11" s="16">
         <v>25.769310000000001</v>
       </c>
-      <c r="K11" s="18">
+      <c r="K11" s="17">
         <v>25.698989999999998</v>
       </c>
     </row>
@@ -4556,8 +4541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AL32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4584,13 +4569,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
       <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
@@ -4668,7 +4653,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C3" s="8">
         <f>LOOKUP($B3,data!$A:$A,data!B:B)</f>
@@ -4678,21 +4663,21 @@
         <f>LOOKUP($B3,data!$A:$A,data!C:C)</f>
         <v>-985</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="21">
         <f>ABS(D3)*$C$16</f>
         <v>24.748743718592966</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="21">
         <f>LOOKUP($B3,data!$A:$A,data!D:D)/1000</f>
         <v>-24.756</v>
       </c>
       <c r="G3" s="7">
         <f>LOOKUP($B3,data!$A:$A,data!J:J)/1000</f>
-        <v>88.02</v>
-      </c>
-      <c r="H3" s="30">
+        <v>132.03</v>
+      </c>
+      <c r="H3" s="19">
         <f>G3/(24*E3)</f>
-        <v>0.14818934010152282</v>
+        <v>0.22228401015228424</v>
       </c>
       <c r="I3">
         <v>2102483898.8800001</v>
@@ -4701,32 +4686,32 @@
         <v>10442175</v>
       </c>
       <c r="K3">
-        <f>LOOKUP($B3,data!$A:$A,data!O:O)</f>
-        <v>3129157077.0999999</v>
+        <f>LOOKUP($B3,data!$A:$A,data!Q:Q)</f>
+        <v>3077005381</v>
       </c>
       <c r="L3">
-        <f>LOOKUP($B3,data!$A:$A,data!P:P)</f>
-        <v>1021235.95017</v>
+        <f>LOOKUP($B3,data!$A:$A,data!R:R)</f>
+        <v>1250952.8899999999</v>
       </c>
       <c r="M3">
         <f>K3-I3</f>
-        <v>1026673178.2199998</v>
+        <v>974521482.11999989</v>
       </c>
       <c r="N3">
         <f>SQRT(POWER(L3,2)+POWER(J3,2))</f>
-        <v>10491994.16681808</v>
+        <v>10516838.967276448</v>
       </c>
       <c r="O3" s="1">
         <f>M3</f>
-        <v>1026673178.2199998</v>
+        <v>974521482.11999989</v>
       </c>
       <c r="P3" s="1">
         <f>2*N3</f>
-        <v>20983988.333636161</v>
+        <v>21033677.934552897</v>
       </c>
       <c r="Q3" s="1">
         <f>O3/C3</f>
-        <v>860581.0379044424</v>
+        <v>816866.28844928741</v>
       </c>
       <c r="R3" s="1"/>
       <c r="S3" s="5"/>
@@ -4754,7 +4739,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C4" s="8">
         <f>LOOKUP($B4,data!$A:$A,data!B:B)</f>
@@ -4762,23 +4747,23 @@
       </c>
       <c r="D4" s="8">
         <f>LOOKUP($B4,data!$A:$A,data!C:C)</f>
-        <v>-754</v>
-      </c>
-      <c r="E4" s="7">
+        <v>-680</v>
+      </c>
+      <c r="E4" s="21">
         <f>ABS(D4)*$C$16</f>
-        <v>18.944723618090453</v>
-      </c>
-      <c r="F4" s="7">
+        <v>17.085427135678394</v>
+      </c>
+      <c r="F4" s="21">
         <f>LOOKUP($B4,data!$A:$A,data!D:D)/1000</f>
-        <v>-18.951000000000001</v>
+        <v>-17.082999999999998</v>
       </c>
       <c r="G4" s="7">
         <f>LOOKUP($B4,data!$A:$A,data!J:J)/1000</f>
-        <v>8.4220000000000006</v>
-      </c>
-      <c r="H4" s="30">
+        <v>0.01</v>
+      </c>
+      <c r="H4" s="19">
         <f>G4/(24*E4)</f>
-        <v>1.8523187444739169E-2</v>
+        <v>2.4387254901960781E-5</v>
       </c>
       <c r="I4">
         <v>1058570571.16</v>
@@ -4787,32 +4772,32 @@
         <v>29664093.298599999</v>
       </c>
       <c r="K4">
-        <f>LOOKUP($B4,data!$A:$A,data!O:O)</f>
-        <v>1941139252.22</v>
+        <f>LOOKUP($B4,data!$A:$A,data!Q:Q)</f>
+        <v>1819594437</v>
       </c>
       <c r="L4">
-        <f>LOOKUP($B4,data!$A:$A,data!P:P)</f>
-        <v>141800.05058099999</v>
+        <f>LOOKUP($B4,data!$A:$A,data!R:R)</f>
+        <v>3395327.2560000001</v>
       </c>
       <c r="M4">
         <f>K4-I4</f>
-        <v>882568681.06000006</v>
+        <v>761023865.84000003</v>
       </c>
       <c r="N4">
         <f>SQRT(POWER(L4,2)+POWER(J4,2))</f>
-        <v>29664432.212371606</v>
+        <v>29857774.170279033</v>
       </c>
       <c r="O4" s="1">
         <f>M4</f>
-        <v>882568681.06000006</v>
+        <v>761023865.84000003</v>
       </c>
       <c r="P4" s="1">
         <f>2*N4</f>
-        <v>59328864.424743213</v>
+        <v>59715548.340558067</v>
       </c>
       <c r="Q4" s="1">
         <f>O4/C4</f>
-        <v>1147683.5904551367</v>
+        <v>989627.91396618995</v>
       </c>
       <c r="R4" s="1"/>
       <c r="S4" s="5"/>
@@ -4840,7 +4825,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C5" s="8">
         <f>LOOKUP($B5,data!$A:$A,data!B:B)</f>
@@ -4850,21 +4835,21 @@
         <f>LOOKUP($B5,data!$A:$A,data!C:C)</f>
         <v>-879</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="21">
         <f>ABS(D5)*$C$16</f>
         <v>22.085427135678394</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="21">
         <f>LOOKUP($B5,data!$A:$A,data!D:D)/1000</f>
         <v>-22.091999999999999</v>
       </c>
       <c r="G5" s="7">
         <f>LOOKUP($B5,data!$A:$A,data!J:J)/1000</f>
-        <v>88.367000000000004</v>
-      </c>
-      <c r="H5" s="30">
+        <v>117.82299999999999</v>
+      </c>
+      <c r="H5" s="19">
         <f>G5/(24*E5)</f>
-        <v>0.16671438187334092</v>
+        <v>0.22228647136897989</v>
       </c>
       <c r="I5">
         <v>1765764570.5999999</v>
@@ -4873,32 +4858,32 @@
         <v>0</v>
       </c>
       <c r="K5">
-        <f>LOOKUP($B5,data!$A:$A,data!O:O)</f>
-        <v>2361366914.3800001</v>
+        <f>LOOKUP($B5,data!$A:$A,data!Q:Q)</f>
+        <v>2309967026</v>
       </c>
       <c r="L5">
-        <f>LOOKUP($B5,data!$A:$A,data!P:P)</f>
-        <v>244351.90852699999</v>
+        <f>LOOKUP($B5,data!$A:$A,data!R:R)</f>
+        <v>24662.697619999999</v>
       </c>
       <c r="M5">
         <f>K5-I5</f>
-        <v>595602343.78000021</v>
+        <v>544202455.4000001</v>
       </c>
       <c r="N5">
         <f>SQRT(POWER(L5,2)+POWER(J5,2))</f>
-        <v>244351.90852699999</v>
+        <v>24662.697619999999</v>
       </c>
       <c r="O5" s="1">
         <f>M5</f>
-        <v>595602343.78000021</v>
+        <v>544202455.4000001</v>
       </c>
       <c r="P5" s="1">
         <f>2*N5</f>
-        <v>488703.81705399998</v>
+        <v>49325.395239999998</v>
       </c>
       <c r="Q5" s="1">
         <f>O5/C5</f>
-        <v>666221.86105145433</v>
+        <v>608727.57874720369</v>
       </c>
       <c r="R5" s="1"/>
       <c r="S5" s="5"/>
@@ -4926,7 +4911,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C6" s="8">
         <f>LOOKUP($B6,data!$A:$A,data!B:B)</f>
@@ -4936,21 +4921,21 @@
         <f>LOOKUP($B6,data!$A:$A,data!C:C)</f>
         <v>-507</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="21">
         <f>ABS(D6)*$C$16</f>
         <v>12.738693467336685</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="21">
         <f>LOOKUP($B6,data!$A:$A,data!D:D)/1000</f>
         <v>-12.743</v>
       </c>
       <c r="G6" s="7">
         <f>LOOKUP($B6,data!$A:$A,data!J:J)/1000</f>
-        <v>5.6639999999999997</v>
-      </c>
-      <c r="H6" s="30">
+        <v>33.981999999999999</v>
+      </c>
+      <c r="H6" s="19">
         <f>G6/(24*E6)</f>
-        <v>1.8526232741617354E-2</v>
+        <v>0.1111508547008547</v>
       </c>
       <c r="I6">
         <v>262400619.102</v>
@@ -4959,32 +4944,32 @@
         <v>553965.52426600002</v>
       </c>
       <c r="K6">
-        <f>LOOKUP($B6,data!$A:$A,data!O:O)</f>
-        <v>1185417154.72</v>
+        <f>LOOKUP($B6,data!$A:$A,data!Q:Q)</f>
+        <v>1172753941</v>
       </c>
       <c r="L6">
-        <f>LOOKUP($B6,data!$A:$A,data!P:P)</f>
-        <v>4245.9820529799999</v>
+        <f>LOOKUP($B6,data!$A:$A,data!R:R)</f>
+        <v>2016.5295349999999</v>
       </c>
       <c r="M6">
         <f>K6-I6</f>
-        <v>923016535.61800003</v>
+        <v>910353321.898</v>
       </c>
       <c r="N6">
         <f>SQRT(POWER(L6,2)+POWER(J6,2))</f>
-        <v>553981.79612591828</v>
+        <v>553969.19451055198</v>
       </c>
       <c r="O6" s="1">
         <f>M6</f>
-        <v>923016535.61800003</v>
+        <v>910353321.898</v>
       </c>
       <c r="P6" s="1">
         <f>2*N6</f>
-        <v>1107963.5922518366</v>
+        <v>1107938.389021104</v>
       </c>
       <c r="Q6" s="1">
         <f>O6/C6</f>
-        <v>1768230.911145594</v>
+        <v>1743971.8810306513</v>
       </c>
       <c r="R6" s="1"/>
       <c r="S6" s="5"/>
@@ -5012,7 +4997,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="C7" s="8">
         <f>LOOKUP($B7,data!$A:$A,data!B:B)</f>
@@ -5020,23 +5005,23 @@
       </c>
       <c r="D7" s="8">
         <f>LOOKUP($B7,data!$A:$A,data!C:C)</f>
-        <v>-185</v>
-      </c>
-      <c r="E7" s="7">
+        <v>-985</v>
+      </c>
+      <c r="E7" s="21">
         <f>ABS(D7)*$C$16</f>
-        <v>4.6482412060301508</v>
-      </c>
-      <c r="F7" s="7">
+        <v>24.748743718592966</v>
+      </c>
+      <c r="F7" s="21">
         <f>LOOKUP($B7,data!$A:$A,data!D:D)/1000</f>
-        <v>-24.756</v>
+        <v>-22.242999999999999</v>
       </c>
       <c r="G7" s="7">
         <f>LOOKUP($B7,data!$A:$A,data!J:J)/1000</f>
-        <v>5545.2460000000001</v>
-      </c>
-      <c r="H7" s="30">
+        <v>0.01</v>
+      </c>
+      <c r="H7" s="19">
         <f>G7/(24*E7)</f>
-        <v>49.707385315315314</v>
+        <v>1.6835871404399323E-5</v>
       </c>
       <c r="I7">
         <v>2742484812.48</v>
@@ -5045,32 +5030,32 @@
         <v>83894741.873400003</v>
       </c>
       <c r="K7">
-        <f>LOOKUP($B7,data!$A:$A,data!O:O)</f>
-        <v>3098642258.48</v>
+        <f>LOOKUP($B7,data!$A:$A,data!Q:Q)</f>
+        <v>2519118573</v>
       </c>
       <c r="L7">
-        <f>LOOKUP($B7,data!$A:$A,data!P:P)</f>
-        <v>84167063.807300001</v>
+        <f>LOOKUP($B7,data!$A:$A,data!R:R)</f>
+        <v>23615885.199999999</v>
       </c>
       <c r="M7">
         <f>K7-I7</f>
-        <v>356157446</v>
+        <v>-223366239.48000002</v>
       </c>
       <c r="N7">
         <f>SQRT(POWER(L7,2)+POWER(J7,2))</f>
-        <v>118837798.46474154</v>
+        <v>87155250.833119601</v>
       </c>
       <c r="O7" s="1">
         <f>M7</f>
-        <v>356157446</v>
+        <v>-223366239.48000002</v>
       </c>
       <c r="P7" s="1">
         <f>2*N7</f>
-        <v>237675596.92948309</v>
+        <v>174310501.6662392</v>
       </c>
       <c r="Q7" s="1">
         <f>O7/C7</f>
-        <v>278248.00468750001</v>
+        <v>-174504.87459375002</v>
       </c>
       <c r="R7" s="1"/>
       <c r="S7" s="5"/>
@@ -5218,8 +5203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Y48"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5796,7 +5781,12 @@
       <c r="O9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="Q9" s="3"/>
+      <c r="P9" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>190</v>
+      </c>
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
@@ -5851,7 +5841,14 @@
       <c r="O10" s="3">
         <v>1193</v>
       </c>
-      <c r="Q10" s="12"/>
+      <c r="P10">
+        <f>H10/SUM(H10,I10,J10,K10,L10)</f>
+        <v>0.78167281836467351</v>
+      </c>
+      <c r="Q10" s="33">
+        <f>G10/SUM(B10:G10)</f>
+        <v>0.2855228127358157</v>
+      </c>
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
@@ -5906,7 +5903,14 @@
       <c r="O11" s="3">
         <v>769</v>
       </c>
-      <c r="Q11" s="12"/>
+      <c r="P11">
+        <f t="shared" ref="P11:P14" si="0">H11/SUM(H11,I11,J11,K11,L11)</f>
+        <v>0.76696460034902836</v>
+      </c>
+      <c r="Q11" s="33">
+        <f t="shared" ref="Q11:Q14" si="1">G11/SUM(B11:G11)</f>
+        <v>0.32405862406832026</v>
+      </c>
       <c r="R11" s="3"/>
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
@@ -5961,7 +5965,14 @@
       <c r="O12" s="3">
         <v>894</v>
       </c>
-      <c r="Q12" s="12"/>
+      <c r="P12">
+        <f t="shared" si="0"/>
+        <v>0.73662650050144862</v>
+      </c>
+      <c r="Q12" s="33">
+        <f t="shared" si="1"/>
+        <v>0.3582399572723477</v>
+      </c>
       <c r="R12" s="3"/>
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
@@ -6016,7 +6027,14 @@
       <c r="O13" s="3">
         <v>522</v>
       </c>
-      <c r="Q13" s="12"/>
+      <c r="P13">
+        <f t="shared" si="0"/>
+        <v>0.76242670307182991</v>
+      </c>
+      <c r="Q13" s="33">
+        <f t="shared" si="1"/>
+        <v>0.31418596732852405</v>
+      </c>
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
@@ -6071,7 +6089,14 @@
       <c r="O14" s="3">
         <v>1280</v>
       </c>
-      <c r="Q14" s="12"/>
+      <c r="P14">
+        <f t="shared" si="0"/>
+        <v>0.72229381664525028</v>
+      </c>
+      <c r="Q14" s="33">
+        <f t="shared" si="1"/>
+        <v>0.48807933456014596</v>
+      </c>
       <c r="R14" s="3"/>
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
@@ -6096,8 +6121,14 @@
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
+      <c r="P15" s="3">
+        <f>AVERAGE(P10:P14)</f>
+        <v>0.75399688778644613</v>
+      </c>
+      <c r="Q15" s="3">
+        <f>AVERAGE(Q10:Q14)</f>
+        <v>0.35401733919303069</v>
+      </c>
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
@@ -6111,55 +6142,55 @@
         <v>17</v>
       </c>
       <c r="B16" s="3" t="str">
-        <f t="shared" ref="B16:N16" si="0">B9</f>
+        <f t="shared" ref="B16:N16" si="2">B9</f>
         <v>HTSE CAPEX</v>
       </c>
       <c r="C16" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>HTSE OM</v>
       </c>
       <c r="D16" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Cap Market</v>
       </c>
       <c r="E16" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>FT CAPEX</v>
       </c>
       <c r="F16" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>FT OM</v>
       </c>
       <c r="G16" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>CO2</v>
       </c>
       <c r="H16" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>H2 PTC</v>
       </c>
       <c r="I16" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Electricity sales</v>
       </c>
       <c r="J16" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Naphta</v>
       </c>
       <c r="K16" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Diesel</v>
       </c>
       <c r="L16" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Jet fuel</v>
       </c>
       <c r="M16" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Storage CAPEX</v>
       </c>
       <c r="N16" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>BAU NPV</v>
       </c>
       <c r="O16" s="3"/>
@@ -6179,55 +6210,55 @@
         <v>Braidwood</v>
       </c>
       <c r="B17" s="11">
-        <f t="shared" ref="B17:N17" si="1">B10/$O10</f>
+        <f t="shared" ref="B17:N17" si="3">B10/$O10</f>
         <v>-553126.8164291702</v>
       </c>
       <c r="C17" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-419125.17183570832</v>
       </c>
       <c r="D17" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-237793.27242246439</v>
       </c>
       <c r="E17" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-217729.70326906958</v>
       </c>
       <c r="F17" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-193469.74266554904</v>
       </c>
       <c r="G17" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-647889.61357921211</v>
       </c>
       <c r="H17" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4006950.5959765296</v>
       </c>
       <c r="I17" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>152.03772003352893</v>
       </c>
       <c r="J17" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>242545.69991617769</v>
       </c>
       <c r="K17" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>278932.82145850797</v>
       </c>
       <c r="L17" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>597541.31181894382</v>
       </c>
       <c r="M17" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-4.1911148365465216</v>
       </c>
       <c r="N17" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1762350.2924392289</v>
       </c>
       <c r="O17" s="3"/>
@@ -6247,55 +6278,55 @@
         <v>Cooper</v>
       </c>
       <c r="B18" s="11">
-        <f t="shared" ref="B18:N18" si="2">B11/$O11</f>
+        <f t="shared" ref="B18:N18" si="4">B11/$O11</f>
         <v>-579586.98309492844</v>
       </c>
       <c r="C18" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-421811.55266579974</v>
       </c>
       <c r="D18" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-237782.28088426529</v>
       </c>
       <c r="E18" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-258735.22236671002</v>
       </c>
       <c r="F18" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-302197.61378413526</v>
       </c>
       <c r="G18" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-863007.31729518855</v>
       </c>
       <c r="H18" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3978814.4707412221</v>
       </c>
       <c r="I18" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>191.19765929778933</v>
       </c>
       <c r="J18" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>227785.84265279584</v>
       </c>
       <c r="K18" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>347002.42912873864</v>
       </c>
       <c r="L18" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>633948.06111833546</v>
       </c>
       <c r="M18" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-6.5019505851755524</v>
       </c>
       <c r="N18" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1376554.7089206763</v>
       </c>
       <c r="O18" s="3"/>
@@ -6315,55 +6346,55 @@
         <v>Davis-Besse</v>
       </c>
       <c r="B19" s="11">
-        <f t="shared" ref="B19:N19" si="3">B12/$O12</f>
+        <f t="shared" ref="B19:N19" si="5">B12/$O12</f>
         <v>-591453.38366890384</v>
       </c>
       <c r="C19" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-437315.95413870248</v>
       </c>
       <c r="D19" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-237786.60514541387</v>
       </c>
       <c r="E19" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-252853.09507829978</v>
       </c>
       <c r="F19" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-264433.06599552574</v>
       </c>
       <c r="G19" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-995767.07270693511</v>
       </c>
       <c r="H19" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3989837.3255033558</v>
       </c>
       <c r="I19" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>257.88031319910516</v>
       </c>
       <c r="J19" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>384648.35011185682</v>
       </c>
       <c r="K19" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>361865.51677852351</v>
       </c>
       <c r="L19" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>679755.01789709169</v>
       </c>
       <c r="M19" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-5.592841163310962</v>
       </c>
       <c r="N19" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1975128.155033557</v>
       </c>
       <c r="O19" s="3"/>
@@ -6383,55 +6414,55 @@
         <v>Prairie-Island</v>
       </c>
       <c r="B20" s="11">
-        <f t="shared" ref="B20:N20" si="4">B13/$O13</f>
+        <f t="shared" ref="B20:N20" si="6">B13/$O13</f>
         <v>-590616.94827586203</v>
       </c>
       <c r="C20" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-412464.09578544059</v>
       </c>
       <c r="D20" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-237767.64750957856</v>
       </c>
       <c r="E20" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-294884.21072796936</v>
       </c>
       <c r="F20" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-443235.20881226053</v>
       </c>
       <c r="G20" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-906607.3026819923</v>
       </c>
       <c r="H20" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3941392.3122605365</v>
       </c>
       <c r="I20" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>8852.015325670498</v>
       </c>
       <c r="J20" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>321981.70689655171</v>
       </c>
       <c r="K20" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>329515.99042145594</v>
       </c>
       <c r="L20" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>567794.00574712642</v>
       </c>
       <c r="M20" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-33524.904214559385</v>
       </c>
       <c r="N20" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>502683.17835632182</v>
       </c>
       <c r="O20" s="3"/>
@@ -6451,55 +6482,55 @@
         <v>STP</v>
       </c>
       <c r="B21" s="11">
-        <f t="shared" ref="B21:N21" si="5">B14/$O14</f>
+        <f t="shared" ref="B21:N21" si="7">B14/$O14</f>
         <v>-574915.96484375</v>
       </c>
       <c r="C21" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-430391.65546874999</v>
       </c>
       <c r="D21" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-237794.62734375001</v>
       </c>
       <c r="E21" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-221802.75234375001</v>
       </c>
       <c r="F21" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-184689.96953125001</v>
       </c>
       <c r="G21" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-1572769.51171875</v>
       </c>
       <c r="H21" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4010361.7476562499</v>
       </c>
       <c r="I21" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>183580.90156249999</v>
       </c>
       <c r="J21" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>234962.76250000001</v>
       </c>
       <c r="K21" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>408207.85234375001</v>
       </c>
       <c r="L21" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>715144.91015625</v>
       </c>
       <c r="M21" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-156250</v>
       </c>
       <c r="N21" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2142566.2597500002</v>
       </c>
       <c r="O21" s="3"/>
@@ -6581,7 +6612,7 @@
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
+      <c r="P24" s="32"/>
       <c r="Q24" s="3"/>
       <c r="R24" s="3"/>
       <c r="S24" s="3"/>
@@ -7226,7 +7257,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7673,10 +7704,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:AC16"/>
+  <dimension ref="A1:AE6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7685,97 +7716,103 @@
     <col min="15" max="15" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" t="s">
         <v>104</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" t="s">
         <v>105</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" t="s">
         <v>107</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" t="s">
         <v>108</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" t="s">
         <v>109</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" t="s">
         <v>110</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="J1" t="s">
         <v>111</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="K1" t="s">
+        <v>187</v>
+      </c>
+      <c r="L1" t="s">
+        <v>188</v>
+      </c>
+      <c r="M1" t="s">
         <v>112</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="N1" t="s">
         <v>113</v>
       </c>
-      <c r="M1" s="19" t="s">
+      <c r="O1" t="s">
         <v>114</v>
       </c>
-      <c r="N1" s="19" t="s">
+      <c r="P1" t="s">
         <v>115</v>
       </c>
-      <c r="O1" s="19" t="s">
+      <c r="Q1" t="s">
         <v>116</v>
       </c>
-      <c r="P1" s="19" t="s">
+      <c r="R1" t="s">
         <v>117</v>
       </c>
-      <c r="Q1" s="19" t="s">
+      <c r="S1" t="s">
         <v>118</v>
       </c>
-      <c r="R1" s="19" t="s">
+      <c r="T1" t="s">
         <v>119</v>
       </c>
-      <c r="S1" s="19" t="s">
+      <c r="U1" t="s">
         <v>120</v>
       </c>
-      <c r="T1" s="19" t="s">
+      <c r="V1" t="s">
         <v>121</v>
       </c>
-      <c r="U1" s="19" t="s">
+      <c r="W1" t="s">
         <v>122</v>
       </c>
-      <c r="V1" s="19" t="s">
+      <c r="X1" t="s">
         <v>123</v>
       </c>
-      <c r="W1" s="19" t="s">
+      <c r="Y1" t="s">
         <v>124</v>
       </c>
-      <c r="X1" s="19" t="s">
+      <c r="Z1" t="s">
         <v>125</v>
       </c>
-      <c r="Y1" s="19" t="s">
+      <c r="AA1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AD1" t="s">
         <v>126</v>
       </c>
-      <c r="Z1" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="AA1" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="AB1" s="19" t="s">
+      <c r="AE1" t="s">
         <v>129</v>
       </c>
-      <c r="AC1" s="19" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
         <v>135</v>
       </c>
       <c r="B2">
@@ -7790,1323 +7827,463 @@
       <c r="E2">
         <v>-14.9</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="20">
         <v>-9.9999999999999997E+199</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="20">
         <v>-9.9999999999999997E+199</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="20">
         <v>-9.9999999999999997E+199</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="20">
         <v>-9.9999999999999997E+199</v>
       </c>
       <c r="J2">
-        <v>77017</v>
-      </c>
-      <c r="K2" t="s">
+        <v>132030</v>
+      </c>
+      <c r="K2" s="20">
+        <v>9.9999999999999997E+199</v>
+      </c>
+      <c r="L2" s="20">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="M2" t="s">
         <v>132</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>131</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>133</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>134</v>
       </c>
-      <c r="O2">
-        <v>3336092227.0700002</v>
-      </c>
-      <c r="P2">
-        <v>1983077.5942200001</v>
-      </c>
       <c r="Q2">
-        <v>3335944003.4299998</v>
+        <v>3077005381</v>
       </c>
       <c r="R2">
-        <v>3338354777.1599998</v>
+        <v>1250952.8899999999</v>
       </c>
       <c r="S2">
-        <v>3334126124.25</v>
+        <v>3076581548</v>
       </c>
       <c r="T2">
-        <v>3334222303.9699998</v>
+        <v>3078804133</v>
       </c>
       <c r="U2">
-        <v>3338169663.25</v>
+        <v>3076054296</v>
       </c>
       <c r="V2">
+        <v>3076086510</v>
+      </c>
+      <c r="W2">
+        <v>3078517620</v>
+      </c>
+      <c r="X2">
         <v>4</v>
       </c>
-      <c r="W2">
-        <v>3932596744690</v>
-      </c>
-      <c r="X2">
-        <v>64</v>
-      </c>
-      <c r="Y2">
-        <v>5.1726977069700003E-2</v>
+      <c r="Y2" s="20">
+        <v>1560000000000</v>
       </c>
       <c r="Z2">
-        <v>3.1933618888500001E-4</v>
+        <v>11</v>
       </c>
       <c r="AA2">
-        <v>0.111122894195</v>
-      </c>
-      <c r="AB2">
-        <v>5.5555555555600003E-2</v>
+        <v>3.42925E-4</v>
+      </c>
+      <c r="AB2" s="20">
+        <v>4.1299999999999998E-14</v>
       </c>
       <c r="AC2">
-        <v>4.6198115829499997E-13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A3" s="19" t="s">
-        <v>136</v>
+        <v>0.111107698</v>
+      </c>
+      <c r="AD2">
+        <v>5.5555555999999999E-2</v>
+      </c>
+      <c r="AE2">
+        <v>5.5555555999999999E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A3" s="18" t="s">
+        <v>138</v>
       </c>
       <c r="B3">
-        <v>1193</v>
+        <v>769</v>
       </c>
       <c r="C3">
-        <v>-985</v>
+        <v>-680</v>
       </c>
       <c r="D3">
-        <v>-24756</v>
+        <v>-17083</v>
       </c>
       <c r="E3">
         <v>-14.9</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="20">
         <v>-9.9999999999999997E+199</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="20">
         <v>-9.9999999999999997E+199</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="20">
         <v>-9.9999999999999997E+199</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="20">
         <v>-9.9999999999999997E+199</v>
       </c>
       <c r="J3">
-        <v>11002</v>
-      </c>
-      <c r="K3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="20">
+        <v>9.9999999999999997E+199</v>
+      </c>
+      <c r="L3" s="20">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="M3" t="s">
         <v>132</v>
       </c>
-      <c r="L3" t="s">
-        <v>131</v>
-      </c>
-      <c r="M3" t="s">
-        <v>133</v>
-      </c>
       <c r="N3" t="s">
+        <v>136</v>
+      </c>
+      <c r="O3" t="s">
+        <v>137</v>
+      </c>
+      <c r="P3" t="s">
         <v>134</v>
       </c>
-      <c r="O3">
-        <v>2927999270.48</v>
-      </c>
-      <c r="P3">
-        <v>2252291.3544100001</v>
-      </c>
       <c r="Q3">
-        <v>2928483762.7199998</v>
+        <v>1819594437</v>
       </c>
       <c r="R3">
-        <v>2930184602.73</v>
+        <v>3395327.2560000001</v>
       </c>
       <c r="S3">
-        <v>2924844953.7399998</v>
+        <v>1821097713</v>
       </c>
       <c r="T3">
-        <v>2925374483.52</v>
+        <v>1821631815</v>
       </c>
       <c r="U3">
-        <v>2929945768.29</v>
+        <v>1814550504</v>
       </c>
       <c r="V3">
+        <v>1815459647</v>
+      </c>
+      <c r="W3">
+        <v>1821624639</v>
+      </c>
+      <c r="X3">
         <v>4</v>
       </c>
-      <c r="W3">
-        <v>5072816345140</v>
-      </c>
-      <c r="X3">
-        <v>10</v>
-      </c>
-      <c r="Y3">
-        <v>5.1726977069700003E-2</v>
+      <c r="Y3" s="20">
+        <v>11500000000000</v>
       </c>
       <c r="Z3">
-        <v>3.19191069053E-4</v>
+        <v>102</v>
       </c>
       <c r="AA3">
-        <v>0.111072395265</v>
+        <v>0.111360239</v>
       </c>
       <c r="AB3">
-        <v>5.5555555555600003E-2</v>
+        <v>0.111111111</v>
       </c>
       <c r="AC3">
-        <v>4.6198115829499997E-13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A4" s="19" t="s">
-        <v>137</v>
+        <v>5.5554106999999998E-2</v>
+      </c>
+      <c r="AD3" s="20">
+        <v>2.79E-14</v>
+      </c>
+      <c r="AE3">
+        <v>6.8739099999999998E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A4" s="18" t="s">
+        <v>141</v>
       </c>
       <c r="B4">
-        <v>1193</v>
+        <v>894</v>
       </c>
       <c r="C4">
-        <v>-985</v>
+        <v>-879</v>
       </c>
       <c r="D4">
-        <v>-24756</v>
+        <v>-22092</v>
       </c>
       <c r="E4">
         <v>-14.9</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="20">
         <v>-9.9999999999999997E+199</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="20">
         <v>-9.9999999999999997E+199</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="20">
         <v>-9.9999999999999997E+199</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="20">
         <v>-9.9999999999999997E+199</v>
       </c>
       <c r="J4">
-        <v>88020</v>
-      </c>
-      <c r="K4" t="s">
+        <v>117823</v>
+      </c>
+      <c r="K4" s="20">
+        <v>9.9999999999999997E+199</v>
+      </c>
+      <c r="L4" s="20">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="M4" t="s">
         <v>132</v>
       </c>
-      <c r="L4" t="s">
-        <v>131</v>
-      </c>
-      <c r="M4" t="s">
-        <v>133</v>
-      </c>
       <c r="N4" t="s">
+        <v>139</v>
+      </c>
+      <c r="O4" t="s">
+        <v>140</v>
+      </c>
+      <c r="P4" t="s">
         <v>134</v>
       </c>
-      <c r="O4">
-        <v>3129157077.0999999</v>
-      </c>
-      <c r="P4">
-        <v>1021235.95017</v>
-      </c>
       <c r="Q4">
-        <v>3129193928.4299998</v>
+        <v>2309967026</v>
       </c>
       <c r="R4">
-        <v>3130347189.9299998</v>
+        <v>24662.697619999999</v>
       </c>
       <c r="S4">
-        <v>3127893261.6399999</v>
+        <v>2309974733</v>
       </c>
       <c r="T4">
-        <v>3128052793.23</v>
+        <v>2309985767</v>
       </c>
       <c r="U4">
-        <v>3130209769.1300001</v>
+        <v>2309932869</v>
       </c>
       <c r="V4">
+        <v>2309937694</v>
+      </c>
+      <c r="W4">
+        <v>2309985566</v>
+      </c>
+      <c r="X4">
         <v>4</v>
       </c>
-      <c r="W4">
-        <v>1042922865930</v>
-      </c>
-      <c r="X4">
-        <v>73</v>
-      </c>
       <c r="Y4">
-        <v>5.1726977069700003E-2</v>
+        <v>608248654</v>
       </c>
       <c r="Z4">
-        <v>3.1933618888500001E-4</v>
+        <v>5.5555555999999999E-2</v>
       </c>
       <c r="AA4">
-        <v>0.111122894195</v>
+        <v>5.5415617E-2</v>
       </c>
       <c r="AB4">
-        <v>5.5555555555600003E-2</v>
+        <v>3.42061E-4</v>
       </c>
       <c r="AC4">
-        <v>4.6198115829499997E-13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A5" s="19" t="s">
-        <v>140</v>
+        <v>0.111107549</v>
+      </c>
+      <c r="AD4">
+        <v>11</v>
+      </c>
+      <c r="AE4" s="20">
+        <v>5.9499999999999999E-14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A5" s="18" t="s">
+        <v>144</v>
       </c>
       <c r="B5">
-        <v>769</v>
+        <v>522</v>
       </c>
       <c r="C5">
-        <v>-754</v>
+        <v>-507</v>
       </c>
       <c r="D5">
-        <v>-18951</v>
+        <v>-12743</v>
       </c>
       <c r="E5">
         <v>-14.9</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="20">
         <v>-9.9999999999999997E+199</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="20">
         <v>-9.9999999999999997E+199</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="20">
         <v>-9.9999999999999997E+199</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="20">
         <v>-9.9999999999999997E+199</v>
       </c>
       <c r="J5">
-        <v>75802</v>
-      </c>
-      <c r="K5" t="s">
+        <v>33982</v>
+      </c>
+      <c r="K5" s="20">
+        <v>9.9999999999999997E+199</v>
+      </c>
+      <c r="L5" s="20">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="M5" t="s">
         <v>132</v>
       </c>
-      <c r="L5" t="s">
-        <v>138</v>
-      </c>
-      <c r="M5" t="s">
-        <v>139</v>
-      </c>
       <c r="N5" t="s">
+        <v>142</v>
+      </c>
+      <c r="O5" t="s">
+        <v>143</v>
+      </c>
+      <c r="P5" t="s">
         <v>134</v>
       </c>
-      <c r="O5">
-        <v>2107073824.25</v>
-      </c>
-      <c r="P5">
-        <v>489213.65802099998</v>
-      </c>
       <c r="Q5">
-        <v>2107275411.9100001</v>
+        <v>1172753941</v>
       </c>
       <c r="R5">
-        <v>2107394878.5</v>
+        <v>2016.5295349999999</v>
       </c>
       <c r="S5">
-        <v>2106349594.6700001</v>
+        <v>1172754138</v>
       </c>
       <c r="T5">
-        <v>2106478332.25</v>
+        <v>1172756136</v>
       </c>
       <c r="U5">
-        <v>2107387093.52</v>
+        <v>1172751353</v>
       </c>
       <c r="V5">
+        <v>1172751688</v>
+      </c>
+      <c r="W5">
+        <v>1172755919</v>
+      </c>
+      <c r="X5">
         <v>4</v>
       </c>
-      <c r="W5">
-        <v>239330003195</v>
-      </c>
-      <c r="X5">
-        <v>91</v>
-      </c>
       <c r="Y5">
-        <v>5.5555555555600003E-2</v>
+        <v>4066391.3670000001</v>
       </c>
       <c r="Z5">
-        <v>1.7071236352900001E-4</v>
+        <v>5.5545076999999998E-2</v>
       </c>
       <c r="AA5">
-        <v>5.55599535571E-2</v>
-      </c>
-      <c r="AB5">
-        <v>5.5306427503699997E-2</v>
+        <v>5.5687203999999997E-2</v>
+      </c>
+      <c r="AB5" s="20">
+        <v>7.3100000000000002E-13</v>
       </c>
       <c r="AC5">
-        <v>1.1730894620700001E-12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
-        <v>141</v>
+        <v>11</v>
+      </c>
+      <c r="AD5">
+        <v>3.4364500000000001E-4</v>
+      </c>
+      <c r="AE5">
+        <v>0.111098577</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A6" s="18" t="s">
+        <v>147</v>
       </c>
       <c r="B6">
-        <v>769</v>
+        <v>1280</v>
       </c>
       <c r="C6">
-        <v>-754</v>
+        <v>-985</v>
       </c>
       <c r="D6">
-        <v>-18951</v>
+        <v>-22243</v>
       </c>
       <c r="E6">
         <v>-14.9</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="20">
         <v>-9.9999999999999997E+199</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="20">
         <v>-9.9999999999999997E+199</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="20">
         <v>-9.9999999999999997E+199</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="20">
         <v>-9.9999999999999997E+199</v>
       </c>
       <c r="J6">
-        <v>8422</v>
-      </c>
-      <c r="K6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="20">
+        <v>9.9999999999999997E+199</v>
+      </c>
+      <c r="L6" s="20">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="M6" t="s">
         <v>132</v>
       </c>
-      <c r="L6" t="s">
-        <v>138</v>
-      </c>
-      <c r="M6" t="s">
-        <v>139</v>
-      </c>
       <c r="N6" t="s">
+        <v>145</v>
+      </c>
+      <c r="O6" t="s">
+        <v>146</v>
+      </c>
+      <c r="P6" t="s">
         <v>134</v>
       </c>
-      <c r="O6">
-        <v>1779039664.3299999</v>
-      </c>
-      <c r="P6">
-        <v>123410.82367899999</v>
-      </c>
       <c r="Q6">
-        <v>1779043416.78</v>
+        <v>2519118573</v>
       </c>
       <c r="R6">
-        <v>1779150445.02</v>
+        <v>23615885.199999999</v>
       </c>
       <c r="S6">
-        <v>1778921378.75</v>
+        <v>2526298656</v>
       </c>
       <c r="T6">
-        <v>1778924911.6600001</v>
+        <v>2554257344</v>
       </c>
       <c r="U6">
-        <v>1779149163.5699999</v>
+        <v>2478346555</v>
       </c>
       <c r="V6">
-        <v>4</v>
+        <v>2481978468</v>
       </c>
       <c r="W6">
-        <v>15230231401.200001</v>
+        <v>2547880238</v>
       </c>
       <c r="X6">
-        <v>11</v>
-      </c>
-      <c r="Y6">
-        <v>5.5555555555600003E-2</v>
-      </c>
-      <c r="Z6">
-        <v>3.4124229874200001E-4</v>
+        <v>10</v>
+      </c>
+      <c r="Y6" s="20">
+        <v>558000000000000</v>
+      </c>
+      <c r="Z6" s="20">
+        <v>5.9100000000000002E-15</v>
       </c>
       <c r="AA6">
-        <v>0.111060534093</v>
+        <v>5.5555555999999999E-2</v>
       </c>
       <c r="AB6">
-        <v>5.5306427503699997E-2</v>
+        <v>5.5555040999999999E-2</v>
       </c>
       <c r="AC6">
-        <v>1.1730894620700001E-12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="B7">
-        <v>769</v>
-      </c>
-      <c r="C7">
-        <v>-754</v>
-      </c>
-      <c r="D7">
-        <v>-18951</v>
-      </c>
-      <c r="E7">
-        <v>-14.9</v>
-      </c>
-      <c r="F7">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="G7">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="H7">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="I7">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="J7">
-        <v>8422</v>
-      </c>
-      <c r="K7" t="s">
-        <v>132</v>
-      </c>
-      <c r="L7" t="s">
-        <v>138</v>
-      </c>
-      <c r="M7" t="s">
-        <v>139</v>
-      </c>
-      <c r="N7" t="s">
-        <v>134</v>
-      </c>
-      <c r="O7">
-        <v>1941139252.22</v>
-      </c>
-      <c r="P7">
-        <v>141800.05058099999</v>
-      </c>
-      <c r="Q7">
-        <v>1941202502.8699999</v>
-      </c>
-      <c r="R7">
-        <v>1941224855.4200001</v>
-      </c>
-      <c r="S7">
-        <v>1940927147.71</v>
-      </c>
-      <c r="T7">
-        <v>1940968232.5899999</v>
-      </c>
-      <c r="U7">
-        <v>1941221720.9300001</v>
-      </c>
-      <c r="V7">
-        <v>4</v>
-      </c>
-      <c r="W7">
-        <v>20107254344.799999</v>
-      </c>
-      <c r="X7">
-        <v>11</v>
-      </c>
-      <c r="Y7">
-        <v>5.5555555555600003E-2</v>
-      </c>
-      <c r="Z7">
-        <v>3.4124229874200001E-4</v>
-      </c>
-      <c r="AA7">
-        <v>0.111060534093</v>
-      </c>
-      <c r="AB7">
-        <v>5.5306427503699997E-2</v>
-      </c>
-      <c r="AC7">
-        <v>1.1730894620700001E-12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A8" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="B8">
-        <v>894</v>
-      </c>
-      <c r="C8">
-        <v>-879</v>
-      </c>
-      <c r="D8">
-        <v>-22092</v>
-      </c>
-      <c r="E8">
-        <v>-14.9</v>
-      </c>
-      <c r="F8">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="G8">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="H8">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="I8">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="J8">
-        <v>88367</v>
-      </c>
-      <c r="K8" t="s">
-        <v>132</v>
-      </c>
-      <c r="L8" t="s">
-        <v>143</v>
-      </c>
-      <c r="M8" t="s">
-        <v>144</v>
-      </c>
-      <c r="N8" t="s">
-        <v>134</v>
-      </c>
-      <c r="O8">
-        <v>2559932748.4000001</v>
-      </c>
-      <c r="P8">
-        <v>237093.99627599999</v>
-      </c>
-      <c r="Q8">
-        <v>2559903677.4499998</v>
-      </c>
-      <c r="R8">
-        <v>2560244307.3299999</v>
-      </c>
-      <c r="S8">
-        <v>2559679331.3499999</v>
-      </c>
-      <c r="T8">
-        <v>2559705002.6999998</v>
-      </c>
-      <c r="U8">
-        <v>2560201193.4099998</v>
-      </c>
-      <c r="V8">
-        <v>4</v>
-      </c>
-      <c r="W8">
-        <v>56213563070.300003</v>
-      </c>
-      <c r="X8">
-        <v>91</v>
-      </c>
-      <c r="Y8">
-        <v>5.5555555555600003E-2</v>
-      </c>
-      <c r="Z8">
-        <v>1.71045534016E-4</v>
-      </c>
-      <c r="AA8">
-        <v>5.5558699367299999E-2</v>
-      </c>
-      <c r="AB8">
-        <v>5.5415617128500003E-2</v>
-      </c>
-      <c r="AC8">
-        <v>7.1438172031400004E-13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="B9">
-        <v>894</v>
-      </c>
-      <c r="C9">
-        <v>-879</v>
-      </c>
-      <c r="D9">
-        <v>-22092</v>
-      </c>
-      <c r="E9">
-        <v>-14.9</v>
-      </c>
-      <c r="F9">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="G9">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="H9">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="I9">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="J9">
-        <v>9819</v>
-      </c>
-      <c r="K9" t="s">
-        <v>132</v>
-      </c>
-      <c r="L9" t="s">
-        <v>143</v>
-      </c>
-      <c r="M9" t="s">
-        <v>144</v>
-      </c>
-      <c r="N9" t="s">
-        <v>134</v>
-      </c>
-      <c r="O9">
-        <v>2167991412.73</v>
-      </c>
-      <c r="P9">
-        <v>16160.8683843</v>
-      </c>
-      <c r="Q9">
-        <v>2167989637.0799999</v>
-      </c>
-      <c r="R9">
-        <v>2168012793.6900001</v>
-      </c>
-      <c r="S9">
-        <v>2167973583.0900002</v>
-      </c>
-      <c r="T9">
-        <v>2167975834.8099999</v>
-      </c>
-      <c r="U9">
-        <v>2168009476.5799999</v>
-      </c>
-      <c r="V9">
-        <v>4</v>
-      </c>
-      <c r="W9">
-        <v>261173666.935</v>
-      </c>
-      <c r="X9">
-        <v>11</v>
-      </c>
-      <c r="Y9">
-        <v>5.5555555555600003E-2</v>
-      </c>
-      <c r="Z9">
-        <v>3.4193427338999999E-4</v>
-      </c>
-      <c r="AA9">
-        <v>0.11106646898399999</v>
-      </c>
-      <c r="AB9">
-        <v>5.5415617128500003E-2</v>
-      </c>
-      <c r="AC9">
-        <v>7.1438172031400004E-13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="B10">
-        <v>894</v>
-      </c>
-      <c r="C10">
-        <v>-879</v>
-      </c>
-      <c r="D10">
-        <v>-22092</v>
-      </c>
-      <c r="E10">
-        <v>-14.9</v>
-      </c>
-      <c r="F10">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="G10">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="H10">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="I10">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="J10">
-        <v>88367</v>
-      </c>
-      <c r="K10" t="s">
-        <v>132</v>
-      </c>
-      <c r="L10" t="s">
-        <v>143</v>
-      </c>
-      <c r="M10" t="s">
-        <v>144</v>
-      </c>
-      <c r="N10" t="s">
-        <v>134</v>
-      </c>
-      <c r="O10">
-        <v>2361366914.3800001</v>
-      </c>
-      <c r="P10">
-        <v>244351.90852699999</v>
-      </c>
-      <c r="Q10">
-        <v>2361386587.27</v>
-      </c>
-      <c r="R10">
-        <v>2361589985.27</v>
-      </c>
-      <c r="S10">
-        <v>2361104497.73</v>
-      </c>
-      <c r="T10">
-        <v>2361120889.6999998</v>
-      </c>
-      <c r="U10">
-        <v>2361585397.0300002</v>
-      </c>
-      <c r="V10">
-        <v>4</v>
-      </c>
-      <c r="W10">
-        <v>59707855200.599998</v>
-      </c>
-      <c r="X10">
-        <v>91</v>
-      </c>
-      <c r="Y10">
-        <v>5.5555555555600003E-2</v>
-      </c>
-      <c r="Z10">
-        <v>1.71045534016E-4</v>
-      </c>
-      <c r="AA10">
-        <v>5.5558699367299999E-2</v>
-      </c>
-      <c r="AB10">
-        <v>5.5415617128500003E-2</v>
-      </c>
-      <c r="AC10">
-        <v>7.1438172031400004E-13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A11" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="B11">
-        <v>522</v>
-      </c>
-      <c r="C11">
-        <v>-507</v>
-      </c>
-      <c r="D11">
-        <v>-12743</v>
-      </c>
-      <c r="E11">
-        <v>-14.9</v>
-      </c>
-      <c r="F11">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="G11">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="H11">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="I11">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="J11">
-        <v>5664</v>
-      </c>
-      <c r="K11" t="s">
-        <v>132</v>
-      </c>
-      <c r="L11" t="s">
-        <v>148</v>
-      </c>
-      <c r="M11" t="s">
-        <v>149</v>
-      </c>
-      <c r="N11" t="s">
-        <v>134</v>
-      </c>
-      <c r="O11">
-        <v>1301597085.5999999</v>
-      </c>
-      <c r="P11">
-        <v>6488.9017495099997</v>
-      </c>
-      <c r="Q11">
-        <v>1301598903.23</v>
-      </c>
-      <c r="R11">
-        <v>1301602273.9100001</v>
-      </c>
-      <c r="S11">
-        <v>1301588262.03</v>
-      </c>
-      <c r="T11">
-        <v>1301589448.3</v>
-      </c>
-      <c r="U11">
-        <v>1301602178.23</v>
-      </c>
-      <c r="V11">
-        <v>4</v>
-      </c>
-      <c r="W11">
-        <v>42105845.914800003</v>
-      </c>
-      <c r="X11">
-        <v>11</v>
-      </c>
-      <c r="Y11">
-        <v>5.5545077329300002E-2</v>
-      </c>
-      <c r="Z11">
-        <v>3.4343045102700002E-4</v>
-      </c>
-      <c r="AA11">
-        <v>0.111029354054</v>
-      </c>
-      <c r="AB11">
-        <v>5.5687203791500002E-2</v>
-      </c>
-      <c r="AC11">
-        <v>4.3848457759400013E-12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A12" s="19" t="s">
-        <v>151</v>
-      </c>
-      <c r="B12">
-        <v>522</v>
-      </c>
-      <c r="C12">
-        <v>-507</v>
-      </c>
-      <c r="D12">
-        <v>-12743</v>
-      </c>
-      <c r="E12">
-        <v>-14.9</v>
-      </c>
-      <c r="F12">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="G12">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="H12">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="I12">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="J12">
-        <v>5664</v>
-      </c>
-      <c r="K12" t="s">
-        <v>132</v>
-      </c>
-      <c r="L12" t="s">
-        <v>148</v>
-      </c>
-      <c r="M12" t="s">
-        <v>149</v>
-      </c>
-      <c r="N12" t="s">
-        <v>134</v>
-      </c>
-      <c r="O12">
-        <v>1069236981.72</v>
-      </c>
-      <c r="P12">
-        <v>5965.3522204800001</v>
-      </c>
-      <c r="Q12">
-        <v>1069237017.4400001</v>
-      </c>
-      <c r="R12">
-        <v>1069243629.74</v>
-      </c>
-      <c r="S12">
-        <v>1069230262.28</v>
-      </c>
-      <c r="T12">
-        <v>1069230833.03</v>
-      </c>
-      <c r="U12">
-        <v>1069243080.41</v>
-      </c>
-      <c r="V12">
-        <v>4</v>
-      </c>
-      <c r="W12">
-        <v>35585427.114399999</v>
-      </c>
-      <c r="X12">
-        <v>11</v>
-      </c>
-      <c r="Y12">
-        <v>5.5545077329300002E-2</v>
-      </c>
-      <c r="Z12">
-        <v>3.4343045102700002E-4</v>
-      </c>
-      <c r="AA12">
-        <v>0.111029354054</v>
-      </c>
-      <c r="AB12">
-        <v>5.5687203791500002E-2</v>
-      </c>
-      <c r="AC12">
-        <v>4.3848457759400013E-12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A13" s="19" t="s">
-        <v>152</v>
-      </c>
-      <c r="B13">
-        <v>522</v>
-      </c>
-      <c r="C13">
-        <v>-507</v>
-      </c>
-      <c r="D13">
-        <v>-12743</v>
-      </c>
-      <c r="E13">
-        <v>-14.9</v>
-      </c>
-      <c r="F13">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="G13">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="H13">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="I13">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="J13">
-        <v>5664</v>
-      </c>
-      <c r="K13" t="s">
-        <v>132</v>
-      </c>
-      <c r="L13" t="s">
-        <v>148</v>
-      </c>
-      <c r="M13" t="s">
-        <v>149</v>
-      </c>
-      <c r="N13" t="s">
-        <v>134</v>
-      </c>
-      <c r="O13">
-        <v>1185417154.72</v>
-      </c>
-      <c r="P13">
-        <v>4245.9820529799999</v>
-      </c>
-      <c r="Q13">
-        <v>1185415958.3099999</v>
-      </c>
-      <c r="R13">
-        <v>1185423186.8599999</v>
-      </c>
-      <c r="S13">
-        <v>1185413515.3900001</v>
-      </c>
-      <c r="T13">
-        <v>1185413748.05</v>
-      </c>
-      <c r="U13">
-        <v>1185422236.3599999</v>
-      </c>
-      <c r="V13">
-        <v>4</v>
-      </c>
-      <c r="W13">
-        <v>18028363.5942</v>
-      </c>
-      <c r="X13">
-        <v>11</v>
-      </c>
-      <c r="Y13">
-        <v>5.5545077329300002E-2</v>
-      </c>
-      <c r="Z13">
-        <v>3.4343045102700002E-4</v>
-      </c>
-      <c r="AA13">
-        <v>0.111029354054</v>
-      </c>
-      <c r="AB13">
-        <v>5.5687203791500002E-2</v>
-      </c>
-      <c r="AC13">
-        <v>4.3848457759400013E-12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A14" s="19" t="s">
-        <v>155</v>
-      </c>
-      <c r="B14">
-        <v>1280</v>
-      </c>
-      <c r="C14">
-        <v>-185</v>
-      </c>
-      <c r="D14">
-        <v>-24756</v>
-      </c>
-      <c r="E14">
-        <v>-14.9</v>
-      </c>
-      <c r="F14">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="G14">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="H14">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="I14">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="J14">
-        <v>5545246</v>
-      </c>
-      <c r="K14" t="s">
-        <v>132</v>
-      </c>
-      <c r="L14" t="s">
-        <v>153</v>
-      </c>
-      <c r="M14" t="s">
-        <v>154</v>
-      </c>
-      <c r="N14" t="s">
-        <v>134</v>
-      </c>
-      <c r="O14">
-        <v>3800558409.5300002</v>
-      </c>
-      <c r="P14">
-        <v>83871384.113399997</v>
-      </c>
-      <c r="Q14">
-        <v>3783027261.9200001</v>
-      </c>
-      <c r="R14">
-        <v>3957928786.75</v>
-      </c>
-      <c r="S14">
-        <v>3695431083.1700001</v>
-      </c>
-      <c r="T14">
-        <v>3711302425.6799998</v>
-      </c>
-      <c r="U14">
-        <v>3925823652.4000001</v>
-      </c>
-      <c r="V14">
-        <v>10</v>
-      </c>
-      <c r="W14">
-        <v>7034409073090000</v>
-      </c>
-      <c r="X14">
-        <v>69</v>
-      </c>
-      <c r="Y14">
-        <v>5.5555555555600003E-2</v>
-      </c>
-      <c r="Z14">
-        <v>6.8587212819100005E-4</v>
-      </c>
-      <c r="AA14">
-        <v>0.111111284767</v>
-      </c>
-      <c r="AB14">
-        <v>0.111111111111</v>
-      </c>
-      <c r="AC14">
-        <v>5.9062379305599996E-15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A15" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="B15">
-        <v>1280</v>
-      </c>
-      <c r="C15">
-        <v>-885</v>
-      </c>
-      <c r="D15">
-        <v>-24756</v>
-      </c>
-      <c r="E15">
-        <v>-14.9</v>
-      </c>
-      <c r="F15">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="G15">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="H15">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="I15">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="J15">
-        <v>924208</v>
-      </c>
-      <c r="K15" t="s">
-        <v>132</v>
-      </c>
-      <c r="L15" t="s">
-        <v>153</v>
-      </c>
-      <c r="M15" t="s">
-        <v>154</v>
-      </c>
-      <c r="N15" t="s">
-        <v>134</v>
-      </c>
-      <c r="O15">
-        <v>2431731991.6100001</v>
-      </c>
-      <c r="P15">
-        <v>18753758.034000002</v>
-      </c>
-      <c r="Q15">
-        <v>2431035910.5</v>
-      </c>
-      <c r="R15">
-        <v>2458018776.3000002</v>
-      </c>
-      <c r="S15">
-        <v>2400215198.6500001</v>
-      </c>
-      <c r="T15">
-        <v>2406824208.23</v>
-      </c>
-      <c r="U15">
-        <v>2455842868.29</v>
-      </c>
-      <c r="V15">
-        <v>10</v>
-      </c>
-      <c r="W15">
-        <v>351703440399000</v>
-      </c>
-      <c r="X15">
-        <v>12</v>
-      </c>
-      <c r="Y15">
-        <v>5.5555555555600003E-2</v>
-      </c>
-      <c r="Z15">
-        <v>6.8586804653700002E-4</v>
-      </c>
-      <c r="AA15">
-        <v>0.111110623539</v>
-      </c>
-      <c r="AB15">
-        <v>0.111111111111</v>
-      </c>
-      <c r="AC15">
-        <v>5.9062379305599996E-15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A16" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="B16">
-        <v>1280</v>
-      </c>
-      <c r="C16">
-        <v>-185</v>
-      </c>
-      <c r="D16">
-        <v>-24756</v>
-      </c>
-      <c r="E16">
-        <v>-14.9</v>
-      </c>
-      <c r="F16">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="G16">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="H16">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="I16">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="J16">
-        <v>5545246</v>
-      </c>
-      <c r="K16" t="s">
-        <v>132</v>
-      </c>
-      <c r="L16" t="s">
-        <v>153</v>
-      </c>
-      <c r="M16" t="s">
-        <v>154</v>
-      </c>
-      <c r="N16" t="s">
-        <v>134</v>
-      </c>
-      <c r="O16">
-        <v>3098642258.48</v>
-      </c>
-      <c r="P16">
-        <v>84167063.807300001</v>
-      </c>
-      <c r="Q16">
-        <v>3117591964.02</v>
-      </c>
-      <c r="R16">
-        <v>3243056165.0599999</v>
-      </c>
-      <c r="S16">
-        <v>2931314128.54</v>
-      </c>
-      <c r="T16">
-        <v>2972276397.7600002</v>
-      </c>
-      <c r="U16">
-        <v>3207143107.9299998</v>
-      </c>
-      <c r="V16">
-        <v>10</v>
-      </c>
-      <c r="W16">
-        <v>7084094629940000</v>
-      </c>
-      <c r="X16">
-        <v>69</v>
-      </c>
-      <c r="Y16">
-        <v>5.5555555555600003E-2</v>
-      </c>
-      <c r="Z16">
-        <v>6.8587212819100005E-4</v>
-      </c>
-      <c r="AA16">
-        <v>0.111111284767</v>
-      </c>
-      <c r="AB16">
-        <v>0.111111111111</v>
-      </c>
-      <c r="AC16">
-        <v>5.9062379305599996E-15</v>
+        <v>101</v>
+      </c>
+      <c r="AD6">
+        <v>3.42932E-4</v>
+      </c>
+      <c r="AE6">
+        <v>0.111111111</v>
       </c>
     </row>
   </sheetData>
@@ -9133,40 +8310,40 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="B1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="C1" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="D1" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="E1" t="s">
         <v>28</v>
       </c>
       <c r="F1" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="G1" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="J1" t="s">
         <v>28</v>
       </c>
       <c r="K1" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="L1" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="M1" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="N1" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="Q1" t="s">
         <v>28</v>
@@ -9175,15 +8352,15 @@
         <v>17</v>
       </c>
       <c r="S1" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="T1" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="B2">
         <v>2102483898.8800001</v>
@@ -9208,7 +8385,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="J2" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="K2">
         <v>972148741.11999989</v>
@@ -9226,7 +8403,7 @@
         <v>72</v>
       </c>
       <c r="R2" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="S2">
         <v>-961918169.88000011</v>
@@ -9237,7 +8414,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="B3">
         <v>3129157077.0999999</v>
@@ -9262,7 +8439,7 @@
         <v>1.0170885706250531E-2</v>
       </c>
       <c r="J3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="K3">
         <v>1535805611.8199999</v>
@@ -9280,7 +8457,7 @@
         <v>72</v>
       </c>
       <c r="R3" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="S3">
         <v>-961918169.88000011</v>
@@ -9291,7 +8468,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B4">
         <v>3074632640</v>
@@ -9316,7 +8493,7 @@
         <v>1.0741335212005283E-2</v>
       </c>
       <c r="J4" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="K4">
         <v>895251155.11999989</v>
@@ -9331,10 +8508,10 @@
         <v>10442175.505490299</v>
       </c>
       <c r="Q4" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="R4" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="S4">
         <v>895251155.11999989</v>
@@ -9345,7 +8522,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="B5">
         <v>3742129513.6399999</v>
@@ -9370,7 +8547,7 @@
         <v>6.3685563983665594E-3</v>
       </c>
       <c r="J5" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="K5">
         <v>1488604013.21</v>
@@ -9385,10 +8562,10 @@
         <v>10442175.57572766</v>
       </c>
       <c r="Q5" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="R5" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="S5">
         <v>895251155.11999989</v>
@@ -9399,7 +8576,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="B6">
         <v>3336092227.0700002</v>
@@ -9439,10 +8616,10 @@
         <v>10442175.528010551</v>
       </c>
       <c r="Q6" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="R6" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="S6">
         <v>972148741.11999989</v>
@@ -9453,7 +8630,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="B7">
         <v>2927999270.48</v>
@@ -9478,10 +8655,10 @@
         <v>1.2649280579076208E-2</v>
       </c>
       <c r="Q7" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="R7" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="S7">
         <v>972148741.11999989</v>
@@ -9492,7 +8669,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="B8">
         <v>2997735054</v>
@@ -9517,10 +8694,10 @@
         <v>1.1663962043322037E-2</v>
       </c>
       <c r="Q8" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="R8" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="S8">
         <v>1535805611.8199997</v>
@@ -9531,7 +8708,7 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B9">
         <v>2587092125.7199998</v>
@@ -9556,10 +8733,10 @@
         <v>2.154766454044935E-2</v>
       </c>
       <c r="Q9" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="R9" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="S9">
         <v>1535805611.8199997</v>
@@ -9570,7 +8747,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="B10">
         <v>3591087912.0900002</v>
@@ -9595,10 +8772,10 @@
         <v>7.0147436417121543E-3</v>
       </c>
       <c r="Q10" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="R10" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="S10">
         <v>1488604013.21</v>
@@ -9609,7 +8786,7 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="B11">
         <v>3225675050</v>
@@ -9634,10 +8811,10 @@
         <v>9.2968819824792524E-3</v>
       </c>
       <c r="Q11" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="R11" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="S11">
         <v>1488604013.21</v>
@@ -9648,7 +8825,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="B12">
         <v>1140565729</v>
@@ -9673,10 +8850,10 @@
         <v>-1.4693771749184141E-2</v>
       </c>
       <c r="Q12" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="R12" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="S12">
         <v>1305852886.8399997</v>
@@ -9687,7 +8864,7 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="B13">
         <v>2930351886</v>
@@ -9712,10 +8889,10 @@
         <v>1.2613334119050742E-2</v>
       </c>
       <c r="Q13" t="s">
+        <v>176</v>
+      </c>
+      <c r="R13" t="s">
         <v>186</v>
-      </c>
-      <c r="R13" t="s">
-        <v>196</v>
       </c>
       <c r="S13">
         <v>1305852886.8399997</v>
@@ -9726,7 +8903,7 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="B14">
         <v>3408336785.7199998</v>
@@ -9753,7 +8930,7 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="B15">
         <v>3408425168</v>
@@ -9783,16 +8960,16 @@
         <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C17" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="D17" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="E17" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -9818,7 +8995,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B19">
         <f>E8</f>
@@ -9839,7 +9016,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B20">
         <f>E4</f>
@@ -9860,7 +9037,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="B21">
         <f>E6</f>
@@ -9881,7 +9058,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="B22">
         <f>E10</f>
@@ -9902,7 +9079,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B23">
         <f>E14</f>
@@ -9942,18 +9119,18 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="B1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="C1" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="B2">
         <v>2102483898.8800001</v>
@@ -9964,27 +9141,27 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="B4" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="C4" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="D4" t="s">
         <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="F4" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="B5">
         <v>3408381162.0100002</v>
@@ -10006,7 +9183,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="B6">
         <v>610618098.39999998</v>
@@ -10028,7 +9205,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B7">
         <v>1140565729</v>
@@ -10050,7 +9227,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="B8">
         <v>2930351886</v>
@@ -10072,10 +9249,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="B10" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>